<commit_message>
se ajusta data y tiempos de esperas
</commit_message>
<xml_diff>
--- a/src/test/resources/files/PlantillaPagosMasivos.xlsx
+++ b/src/test/resources/files/PlantillaPagosMasivos.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5714" uniqueCount="1193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5764" uniqueCount="1199">
   <si>
     <t>VehicleDamage</t>
   </si>
@@ -3629,6 +3629,24 @@
   </si>
   <si>
     <t>13072021150827561</t>
+  </si>
+  <si>
+    <t>9210000059234</t>
+  </si>
+  <si>
+    <t>140718</t>
+  </si>
+  <si>
+    <t>15092021080357347</t>
+  </si>
+  <si>
+    <t>SYEA151</t>
+  </si>
+  <si>
+    <t>535312</t>
+  </si>
+  <si>
+    <t>15092021080400373</t>
   </si>
 </sst>
 </file>
@@ -5103,7 +5121,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="31">
-        <v>1187</v>
+        <v>1193</v>
       </c>
       <c r="B2" t="s" s="32">
         <v>1181</v>
@@ -5145,7 +5163,7 @@
         <v>505</v>
       </c>
       <c r="O2" t="s" s="19">
-        <v>1188</v>
+        <v>1194</v>
       </c>
       <c r="P2" t="s" s="19">
         <v>736</v>
@@ -5166,7 +5184,7 @@
         <v>737</v>
       </c>
       <c r="V2" t="s" s="37">
-        <v>1189</v>
+        <v>1195</v>
       </c>
       <c r="X2" t="s" s="4">
         <v>730</v>
@@ -5180,10 +5198,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="31">
-        <v>1187</v>
+        <v>1193</v>
       </c>
       <c r="B3" t="s" s="32">
-        <v>1190</v>
+        <v>1196</v>
       </c>
       <c r="C3" t="s" s="32">
         <v>50</v>
@@ -5222,7 +5240,7 @@
         <v>505</v>
       </c>
       <c r="O3" t="s" s="19">
-        <v>1191</v>
+        <v>1197</v>
       </c>
       <c r="P3" t="s" s="19">
         <v>736</v>
@@ -5243,7 +5261,7 @@
         <v>737</v>
       </c>
       <c r="V3" t="s" s="37">
-        <v>1192</v>
+        <v>1198</v>
       </c>
       <c r="X3" t="s" s="4">
         <v>730</v>

</xml_diff>